<commit_message>
update strategy settings and so files for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/general/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/general/运维事项确认表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1.sh_19_day" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -395,17 +395,15 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>主力合约</t>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>测试新的行情
+上期新行情测试的</t>
     </r>
     <r>
       <rPr>
@@ -415,39 +413,17 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">
-2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>手数</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>(ok)1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">手数
-</t>
+      <t>so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，可以配</t>
     </r>
     <r>
       <rPr>
@@ -457,7 +433,64 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(ok)2.so</t>
+      <t xml:space="preserve">zn
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(ok)更新so
+(ok)更新手数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(ok)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新SO
+(ok)2.更新手数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(ok)1. so
+(ok)2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>手数</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,9 +641,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -634,6 +664,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,13 +1081,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5">
+    <row r="3" spans="1:5" ht="27">
       <c r="A3" s="10"/>
       <c r="B3" s="11">
-        <v>42820</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>31</v>
+        <v>42829</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>24</v>
@@ -1202,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1213,36 +1246,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5">
-      <c r="A2" s="17">
-        <v>42820</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="19" t="s">
+    <row r="2" spans="1:4" ht="56.25">
+      <c r="A2" s="16">
+        <v>42829</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1261,38 +1295,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="40.5">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>42815</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
@@ -1325,24 +1359,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>42815</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
@@ -1361,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1374,31 +1408,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="20">
-        <v>42815</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1422,31 +1442,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42.75" customHeight="1">
-      <c r="A2" s="20">
-        <v>42815</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>27</v>
+      <c r="A2" s="19">
+        <v>42829</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1473,24 +1493,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42.75">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>42815</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C2" t="s">
@@ -1501,88 +1521,88 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1595,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1606,25 +1626,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5">
-      <c r="A2" s="20">
-        <v>42820</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>29</v>
+      <c r="A2" s="19">
+        <v>42829</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -1655,24 +1675,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>42815</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">

</xml_diff>